<commit_message>
tidy up duplicates in stopwords.xlsx
</commit_message>
<xml_diff>
--- a/data/stopwords.xlsx
+++ b/data/stopwords.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://connectqutedu-my.sharepoint.com/personal/whitenm_qut_edu_au/Documents/Git projects/stats_section/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="11" documentId="13_ncr:40009_{247D78DE-F642-45E2-8AC0-5B48667A056B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{1D9ADFB7-DC73-45D2-B787-0CC90E3F94B5}"/>
+  <xr:revisionPtr revIDLastSave="17" documentId="13_ncr:40009_{247D78DE-F642-45E2-8AC0-5B48667A056B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{411B9442-E404-4D3A-84B4-81052AEC64B0}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="stopwords" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="352" uniqueCount="184">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="358" uniqueCount="187">
   <si>
     <t>i</t>
   </si>
@@ -573,6 +573,15 @@
   </si>
   <si>
     <t>stopword</t>
+  </si>
+  <si>
+    <t>use</t>
+  </si>
+  <si>
+    <t>used</t>
+  </si>
+  <si>
+    <t>using</t>
   </si>
 </sst>
 </file>
@@ -1413,10 +1422,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B167"/>
+  <dimension ref="A1:B170"/>
   <sheetViews>
-    <sheetView topLeftCell="A103" workbookViewId="0">
-      <selection activeCell="I132" sqref="I132"/>
+    <sheetView tabSelected="1" topLeftCell="A154" workbookViewId="0">
+      <selection activeCell="H173" sqref="H173"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2761,6 +2770,30 @@
         <v>119</v>
       </c>
     </row>
+    <row r="168" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A168" t="s">
+        <v>184</v>
+      </c>
+      <c r="B168" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="169" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A169" t="s">
+        <v>185</v>
+      </c>
+      <c r="B169" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="170" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A170" t="s">
+        <v>186</v>
+      </c>
+      <c r="B170" t="s">
+        <v>119</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2770,8 +2803,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:B9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I19" sqref="I19"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>